<commit_message>
Added a Labor Budget column to the consolidation and therefore to the Cell Map to be captured.
</commit_message>
<xml_diff>
--- a/Cell Map.xlsx
+++ b/Cell Map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/381a7f7f8544557d/Documents/Programs/AutoConsolidation/Auto Consolidate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaronMelton\OneDrive\Documents\Programs\AutoConsolidation\Auto Consolidate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{F2B98509-37EA-484F-A51E-D1F8B8133B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEFB857B-501E-494D-A9E8-F47B74BD13CA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C64EBE7-BD52-41DF-B9E8-0071E13486DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4027BA0D-4378-4D22-B711-84875D13CA51}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4027BA0D-4378-4D22-B711-84875D13CA51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Source Sheet</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>Ref Drawing(s)</t>
+  </si>
+  <si>
+    <t>G54</t>
+  </si>
+  <si>
+    <t>Labor Budget</t>
   </si>
 </sst>
 </file>
@@ -235,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -244,9 +250,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D81DB93-1D0F-4C15-ADE3-2DDC82CF2218}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,13 +611,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -825,6 +828,17 @@
       </c>
       <c r="C21" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>